<commit_message>
Update radar for S1 2019
</commit_message>
<xml_diff>
--- a/radar.xlsx
+++ b/radar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\clients\mitrais\sources\radar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\internal\bootcamp-java\java-black-belt\java-cert-exam-questions\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7031199-6395-426A-A1D0-2ED1300830DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00D16E1-A765-451F-9F90-1150C78BB628}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="-110" windowWidth="18450" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33225" yWindow="1635" windowWidth="13665" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-S1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -49,15 +49,6 @@
     <t>tools</t>
   </si>
   <si>
-    <t>techniques</t>
-  </si>
-  <si>
-    <t>platforms</t>
-  </si>
-  <si>
-    <t>MongoDB</t>
-  </si>
-  <si>
     <t>JDK 11</t>
   </si>
   <si>
@@ -85,10 +76,29 @@
     <t>&lt;strong&gt;Spring Web Flux&lt;/strong&gt; reactive-stack web framework, it is fully non-blocking, supports &lt;a href="https://www.reactive-streams.org"&gt;Reactive Streams&lt;/a&gt; back pressure, and runs on such servers as Netty, Undertow, and Servlet 3.1+ containers.</t>
   </si>
   <si>
-    <t>Google Cloud Platform</t>
-  </si>
-  <si>
-    <t>Microservices</t>
+    <t>Metrics by Dropwizard</t>
+  </si>
+  <si>
+    <t>Metrics provides a powerful toolkit of ways to measure the behavior of critical components in your production environment</t>
+  </si>
+  <si>
+    <t>Apache Kafka</t>
+  </si>
+  <si>
+    <t>Kafka is used for building real-time data pipelines and streaming apps. It is horizontally scalable, fault-tolerant, fast, and runs in production in thousands of companies.
+A streaming platform has three key capabilities:
+Publish and subscribe to streams of records, similar to a message queue or enterprise messaging system.
+Store streams of records in a fault-tolerant durable way.
+Process streams of records as they occur.
+Kafka is generally used for two broad classes of applications:
+Building real-time streaming data pipelines that reliably get data between systems or applications
+Building real-time streaming applications that transform or react to the streams of data</t>
+  </si>
+  <si>
+    <t>Elasticsearch</t>
+  </si>
+  <si>
+    <t>Elasticsearch is a distributed, RESTful search and analytics engine.</t>
   </si>
 </sst>
 </file>
@@ -572,11 +582,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -935,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -966,7 +979,7 @@
     </row>
     <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -978,15 +991,15 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -995,12 +1008,12 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -1012,15 +1025,15 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -1029,12 +1042,12 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1045,19 +1058,25 @@
       <c r="D6" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1068,10 +1087,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add emerging technologies candidates
</commit_message>
<xml_diff>
--- a/radar.xlsx
+++ b/radar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clients\mitrais\sources\radar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACFAFA5-D494-4091-8D7F-333CE965C68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99D6C6D-2DF4-489B-AD27-6B5F4DD10963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="830" yWindow="-110" windowWidth="18480" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-S2" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -246,6 +246,39 @@
   </si>
   <si>
     <t>Clojure is a dynamic, general-purpose programming language, combining the approachability and interactive development of a scripting language with an efficient and robust infrastructure for multithreaded programming. Clojure is a compiled language, yet remains completely dynamic – every feature supported by Clojure is supported at runtime. Clojure provides easy access to the Java frameworks, with optional type hints and type inference, to ensure that calls to Java can avoid reflection.</t>
+  </si>
+  <si>
+    <t>Progressive Web Apps</t>
+  </si>
+  <si>
+    <t>AWS Amplify</t>
+  </si>
+  <si>
+    <t>Google Cloud Platform</t>
+  </si>
+  <si>
+    <t>Azure Devops</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;PWA features allow to close the gap to native applications and create similar user experiences. Features include&lt;/p&gt;
+&lt;ul&gt;&lt;li&gt;Work offline&lt;/li&gt;
+&lt;li&gt;High performance&lt;/li&gt;
+&lt;li&gt;Background processing in service workers in a separate thread&lt;/li&gt;
+&lt;li&gt;Access to the phone's sensors&lt;/li&gt;
+&lt;li&gt;Support for push notifications&lt;/li&gt;
+&lt;li&gt;An icon on the phone‘s home screen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>A set of products and tools that enables mobile and front-end web developers to build and deploy secure, scalable full stack applications, powered by AWS. With Amplify, you can configure app backends in minutes, connect them to your app in just a few lines of code, and deploy static web apps in three steps.</t>
+  </si>
+  <si>
+    <t>A suite of cloud computing services that runs on the same infrastructure that Google uses internally for its end-user products, such as Google Search, Gmail, file storage, and YouTube.</t>
+  </si>
+  <si>
+    <t>A Software as a service (SaaS) platform from Microsoft that provides an end-to-end DevOps toolchain for developing and deploying software. It also integrates with most leading tools on the market and is a great option for orchestrating a DevOps toolchain.</t>
+  </si>
+  <si>
+    <t>Blazor is a feature of ASP.NET for building interactive web UIs using C# instead of JavaScript. It's real .NET running in the browser on WebAssembly.</t>
   </si>
 </sst>
 </file>
@@ -1098,21 +1131,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F17DE5E-55DD-4A84-BDB3-285BA5B83CDB}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1146,7 +1179,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1180,7 +1213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1197,7 +1230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>57</v>
       </c>
@@ -1214,7 +1247,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1231,7 +1264,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1248,7 +1281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
@@ -1265,7 +1298,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1282,7 +1315,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>63</v>
       </c>
@@ -1299,7 +1332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1316,7 +1349,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
@@ -1333,7 +1366,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
@@ -1350,7 +1383,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1365,6 +1398,91 @@
       </c>
       <c r="E15" s="2" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1381,15 +1499,15 @@
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1423,7 +1541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1440,7 +1558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1457,7 +1575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1474,7 +1592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1491,7 +1609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1508,7 +1626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1542,7 +1660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1559,7 +1677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1576,7 +1694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1593,7 +1711,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1610,7 +1728,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1627,7 +1745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1644,7 +1762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1661,7 +1779,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1678,7 +1796,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -1695,7 +1813,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -1712,7 +1830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -1729,7 +1847,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
@@ -1760,15 +1878,15 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1802,7 +1920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1819,7 +1937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1836,7 +1954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1853,7 +1971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1870,7 +1988,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1887,7 +2005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1904,7 +2022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1921,7 +2039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1938,7 +2056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1955,7 +2073,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1972,7 +2090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1989,7 +2107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -2006,7 +2124,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -2023,7 +2141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -2040,7 +2158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Fix Blazor displayed twice and set Flutter to adopt
</commit_message>
<xml_diff>
--- a/radar.xlsx
+++ b/radar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clients\mitrais\sources\radar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99D6C6D-2DF4-489B-AD27-6B5F4DD10963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2129DB-A21D-4ED6-86B7-FBCD3F08ED9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="79">
   <si>
     <t>name</t>
   </si>
@@ -276,9 +276,6 @@
   </si>
   <si>
     <t>A Software as a service (SaaS) platform from Microsoft that provides an end-to-end DevOps toolchain for developing and deploying software. It also integrates with most leading tools on the market and is a great option for orchestrating a DevOps toolchain.</t>
-  </si>
-  <si>
-    <t>Blazor is a feature of ASP.NET for building interactive web UIs using C# instead of JavaScript. It's real .NET running in the browser on WebAssembly.</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F17DE5E-55DD-4A84-BDB3-285BA5B83CDB}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,7 +1249,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -1466,23 +1463,6 @@
       </c>
       <c r="E19" s="3" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>